<commit_message>
Fixed some examples, Amp classification diagrams
</commit_message>
<xml_diff>
--- a/docs/Examples/Five_min_intro.xlsx
+++ b/docs/Examples/Five_min_intro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB163F79-BA3A-4824-BC31-C766773E2DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41850A15-4296-4F39-928E-C13A7DFDBEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{8F6528E9-49AA-4EB4-BB80-AD36285B293C}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="wrong_header_caps" sheetId="3" r:id="rId3"/>
     <sheet name="no_feot" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1717,10 +1717,13 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
added optoin for FeO and Fe2O3 and petrolog to example
</commit_message>
<xml_diff>
--- a/docs/Examples/Five_min_intro.xlsx
+++ b/docs/Examples/Five_min_intro.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41850A15-4296-4F39-928E-C13A7DFDBEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD2F125-93C2-462E-BD28-535726C6F54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{8F6528E9-49AA-4EB4-BB80-AD36285B293C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="4" xr2:uid="{8F6528E9-49AA-4EB4-BB80-AD36285B293C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Liq_noheader" sheetId="2" r:id="rId2"/>
     <sheet name="wrong_header_caps" sheetId="3" r:id="rId3"/>
     <sheet name="no_feot" sheetId="4" r:id="rId4"/>
+    <sheet name="Feo_Fe2O3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -214,6 +215,9 @@
   </si>
   <si>
     <t>FeO_Liq</t>
+  </si>
+  <si>
+    <t>Fe2O3_Liq</t>
   </si>
 </sst>
 </file>
@@ -571,12 +575,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -718,7 +722,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -789,7 +793,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -860,7 +864,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -931,7 +935,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1015,12 +1019,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1065,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1102,7 +1106,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1143,7 +1147,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1184,7 +1188,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1279,9 +1283,9 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1494,7 +1498,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1636,7 +1640,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1716,16 +1720,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E29D89-A58E-47CE-80D2-3562B27B855C}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1811,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1889,7 +1893,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1930,7 +1934,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1968,6 +1972,285 @@
         <v>0.23</v>
       </c>
       <c r="M6">
+        <v>6.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AB3B65-E880-46F7-A970-3EA0543BC41B}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>51.1</v>
+      </c>
+      <c r="C2">
+        <v>0.93</v>
+      </c>
+      <c r="D2">
+        <v>17.5</v>
+      </c>
+      <c r="E2">
+        <v>8.91</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.18</v>
+      </c>
+      <c r="H2">
+        <v>6.09</v>
+      </c>
+      <c r="I2">
+        <v>11.5</v>
+      </c>
+      <c r="J2">
+        <v>3.53</v>
+      </c>
+      <c r="K2">
+        <v>0.17</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.15</v>
+      </c>
+      <c r="N2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>51.5</v>
+      </c>
+      <c r="C3">
+        <v>1.19</v>
+      </c>
+      <c r="D3">
+        <v>19.2</v>
+      </c>
+      <c r="E3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+      <c r="G3">
+        <v>0.19</v>
+      </c>
+      <c r="H3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>3.72</v>
+      </c>
+      <c r="K3">
+        <v>0.42</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>59.1</v>
+      </c>
+      <c r="C4">
+        <v>0.54</v>
+      </c>
+      <c r="D4">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E4">
+        <v>5.22</v>
+      </c>
+      <c r="F4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.19</v>
+      </c>
+      <c r="H4">
+        <v>3.25</v>
+      </c>
+      <c r="I4">
+        <v>7.45</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>0.88</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0.31</v>
+      </c>
+      <c r="N4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>52.5</v>
+      </c>
+      <c r="C5">
+        <v>0.98</v>
+      </c>
+      <c r="D5">
+        <v>19.2</v>
+      </c>
+      <c r="E5">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="F5">
+        <v>1.2</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
+      </c>
+      <c r="H5">
+        <v>4.99</v>
+      </c>
+      <c r="I5">
+        <v>9.64</v>
+      </c>
+      <c r="J5">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="K5">
+        <v>0.21</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N5">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>56.2</v>
+      </c>
+      <c r="C6">
+        <v>0.34</v>
+      </c>
+      <c r="D6">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E6">
+        <v>5.88</v>
+      </c>
+      <c r="F6">
+        <v>1.3</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>2.58</v>
+      </c>
+      <c r="I6">
+        <v>7.18</v>
+      </c>
+      <c r="J6">
+        <v>6.02</v>
+      </c>
+      <c r="K6">
+        <v>1.02</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.23</v>
+      </c>
+      <c r="N6">
         <v>6.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweaked Rasmussen - linear fit didnt intercept origin, changed to 4th order polynomail
</commit_message>
<xml_diff>
--- a/docs/Examples/Five_min_intro.xlsx
+++ b/docs/Examples/Five_min_intro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD2F125-93C2-462E-BD28-535726C6F54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170FC72-8DBD-4122-8054-77C339A17583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="4" xr2:uid="{8F6528E9-49AA-4EB4-BB80-AD36285B293C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="4" xr2:uid="{8F6528E9-49AA-4EB4-BB80-AD36285B293C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1721,7 +1721,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1985,10 +1985,13 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>